<commit_message>
Limit witdth of name and description columns
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -34,7 +34,7 @@
     <t>norm:inline → "inside inline"</t>
   </si>
   <si>
-    <t>paragraph</t>
+    <t>paragraph-with-a-really-wide-rule-name</t>
   </si>
   <si>
     <t>Here's a description.
@@ -47,7 +47,7 @@
     <t>note_with_2_tags</t>
   </si>
   <si>
-    <t>Here's a one line description.</t>
+    <t>Here's a one line description but it is very wide so should wrap within a cell.</t>
   </si>
   <si>
     <t>parameter</t>
@@ -446,9 +446,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.7109375" bestFit="1" customWidth="1"/>
@@ -481,7 +481,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -501,7 +501,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -515,7 +515,7 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -535,7 +535,7 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -546,7 +546,7 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">

</xml_diff>

<commit_message>
Much improved XLSX format of norm rules
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -22,32 +22,39 @@
     <t>inline</t>
   </si>
   <si>
-    <t>A few words</t>
+    <t>A few words
+inside inline</t>
+  </si>
+  <si>
+    <t>Summary, ["norm:inline"]</t>
   </si>
   <si>
     <t>extension</t>
   </si>
   <si>
-    <t>Zicsr,ABC</t>
-  </si>
-  <si>
-    <t>norm:inline → "inside inline"</t>
+    <t>Zicsr, ABC</t>
   </si>
   <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
   </si>
   <si>
     <t>Here's a description.
-It's got 2 lines.</t>
-  </si>
-  <si>
-    <t>norm:para → "Paragraph anchor"</t>
+It's got 2 lines.
+Paragraph anchor</t>
+  </si>
+  <si>
+    <t>Description, ["norm:para"]</t>
   </si>
   <si>
     <t>note_with_2_tags</t>
   </si>
   <si>
-    <t>Here's a one line description but it is very wide so should wrap within a cell.</t>
+    <t>One line description
+Multi-paragraph note 1
+Multi-paragraph note 3</t>
+  </si>
+  <si>
+    <t>Description, ["norm:note-1", "norm:note-3"]</t>
   </si>
   <si>
     <t>parameter</t>
@@ -56,39 +63,45 @@
     <t>MY_PARAMETER</t>
   </si>
   <si>
-    <t>norm:note-1 → "Multi-paragraph note 1"
-norm:note-3 → "Multi-paragraph note 3"</t>
-  </si>
-  <si>
     <t>desc1</t>
   </si>
   <si>
-    <t>norm:description-item-1 → "Description Item 1"
-norm:description-item-3 → "Description Item 3"</t>
+    <t>Description Item 1
+Description Item 3</t>
+  </si>
+  <si>
+    <t>["norm:description-item-1", "norm:description-item-3"]</t>
   </si>
   <si>
     <t>desc2</t>
   </si>
   <si>
+    <t>rule_with_newlines</t>
+  </si>
+  <si>
+    <t>Here&amp;#8217;s the first line.
+Here&amp;#8217;s the second line.</t>
+  </si>
+  <si>
+    <t>["norm:tag_with_newlines"]</t>
+  </si>
+  <si>
     <t>Chapter Name</t>
   </si>
   <si>
     <t>Rule Name</t>
   </si>
   <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>Rule Definition</t>
+  </si>
+  <si>
+    <t>Rule Definition Sources</t>
   </si>
   <si>
     <t>Kind</t>
   </si>
   <si>
     <t>Instances</t>
-  </si>
-  <si>
-    <t>Tagged Text</t>
   </si>
 </sst>
 </file>
@@ -139,16 +152,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G5" totalsRowShown="0">
-  <autoFilter ref="A1:G5"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0">
+  <autoFilter ref="A1:F6"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
-    <tableColumn id="3" name="Summary"/>
-    <tableColumn id="4" name="Description"/>
+    <tableColumn id="3" name="Rule Definition"/>
+    <tableColumn id="4" name="Rule Definition Sources"/>
     <tableColumn id="5" name="Kind"/>
     <tableColumn id="6" name="Instances"/>
-    <tableColumn id="7" name="Tagged Text"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -439,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,110 +459,126 @@
   <cols>
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: added test cases to test.adoc and updated expected result files
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -35,26 +35,65 @@
     <t>Zicsr, ABC</t>
   </si>
   <si>
+    <t>inline-anchors-in-paragraph</t>
+  </si>
+  <si>
+    <t>Paragraph with inline anchor and something.</t>
+  </si>
+  <si>
+    <t>["norm:paragraph:inline-anchors-in-paragraph"]</t>
+  </si>
+  <si>
+    <t>inline-anchors-in-tagged-paragraph</t>
+  </si>
+  <si>
+    <t>inline anchor</t>
+  </si>
+  <si>
+    <t>["norm:paragraph:inline-anchors-in-paragraph:inline-anchors"]</t>
+  </si>
+  <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
   </si>
   <si>
     <t>Here's a description.
 It's got 2 lines.
-Paragraph anchor</t>
-  </si>
-  <si>
-    <t>Description, ["norm:para"]</t>
+Paragraph without inline anchors</t>
+  </si>
+  <si>
+    <t>Description, ["norm:paragraph:no-inline-anchors-in-paragraph"]</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>["norm:table:anchors-in-cells:entire-table"]</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>["norm:table:no-anchors-in-cells:entire-table"]</t>
+  </si>
+  <si>
+    <t>unordered1</t>
+  </si>
+  <si>
+    <t>Unordered List with anchors:</t>
+  </si>
+  <si>
+    <t>["norm:unordered-list:anchors-in-items:entire-list"]</t>
   </si>
   <si>
     <t>note_with_2_tags</t>
   </si>
   <si>
     <t>One line description
-Multi-paragraph note 1
-Multi-paragraph note 3</t>
-  </si>
-  <si>
-    <t>Description, ["norm:note-1", "norm:note-3"]</t>
+Paragraph 1
+Paragraph 3</t>
+  </si>
+  <si>
+    <t>Description, ["norm:admonition:anchors-in-notes:note1", "norm:admonition:anchors-in-notes:note3"]</t>
   </si>
   <si>
     <t>parameter</t>
@@ -70,7 +109,7 @@
 Description Item 3</t>
   </si>
   <si>
-    <t>["norm:description-item-1", "norm:description-item-3"]</t>
+    <t>["norm:description-list:anchors-in-items:item1", "norm:description-list:anchors-in-items:item3"]</t>
   </si>
   <si>
     <t>desc2</t>
@@ -79,8 +118,7 @@
     <t>rule_with_newlines</t>
   </si>
   <si>
-    <t>Here&amp;#8217;s the first line.
-Here&amp;#8217;s the second line.</t>
+    <t>Here&amp;#8217;s the first line. Here&amp;#8217;s the second line.</t>
   </si>
   <si>
     <t>["norm:tag_with_newlines"]</t>
@@ -152,8 +190,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
+  <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -451,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,22 +505,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -532,25 +570,19 @@
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -558,10 +590,14 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C6" s="1">
+        <f>==
+ cell with anchor
+cell without anchor
+===</f>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -572,13 +608,94 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1">
+        <f>Header 1|Header 2
+==
+Cell in column 1, row 1|Cell in column 2, row 1
+Cell in column 1, row 2|Cell in column 2, row 2
+===</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed #97 and #98
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -35,24 +35,6 @@
     <t>Zicsr, ABC</t>
   </si>
   <si>
-    <t>inline-anchors-in-paragraph</t>
-  </si>
-  <si>
-    <t>Paragraph with inline anchor and something.</t>
-  </si>
-  <si>
-    <t>["norm:paragraph:inline-anchors-in-paragraph"]</t>
-  </si>
-  <si>
-    <t>inline-anchors-in-tagged-paragraph</t>
-  </si>
-  <si>
-    <t>inline anchor</t>
-  </si>
-  <si>
-    <t>["norm:paragraph:inline-anchors-in-paragraph:inline-anchors"]</t>
-  </si>
-  <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
   </si>
   <si>
@@ -61,7 +43,34 @@
 Paragraph without inline anchors</t>
   </si>
   <si>
-    <t>Description, ["norm:paragraph:no-inline-anchors-in-paragraph"]</t>
+    <t>Description, ["norm:paragraph:no-inline-anchors"]</t>
+  </si>
+  <si>
+    <t>inline-anchors-in-paragraph-entire</t>
+  </si>
+  <si>
+    <t>Paragraph with inline anchor and something.</t>
+  </si>
+  <si>
+    <t>["norm:paragraph:inline-anchors:entire"]</t>
+  </si>
+  <si>
+    <t>inline-anchors-in-paragraph-inline-anchor</t>
+  </si>
+  <si>
+    <t>inline anchor</t>
+  </si>
+  <si>
+    <t>["norm:paragraph:inline-anchors:inline-anchor"]</t>
+  </si>
+  <si>
+    <t>rule_with_newlines</t>
+  </si>
+  <si>
+    <t>Here&amp;#8217;s the first line. Here&amp;#8217;s the second line.</t>
+  </si>
+  <si>
+    <t>["norm:paragraph:tag_with_newlines"]</t>
   </si>
   <si>
     <t>table1</t>
@@ -79,7 +88,9 @@
     <t>unordered1</t>
   </si>
   <si>
-    <t>Unordered List with anchors:</t>
+    <t>Item 1
+ Item 2
+Item 3</t>
   </si>
   <si>
     <t>["norm:unordered-list:anchors-in-items:entire-list"]</t>
@@ -105,23 +116,14 @@
     <t>desc1</t>
   </si>
   <si>
-    <t>Description Item 1
-Description Item 3</t>
+    <t>Item 1
+Item 3</t>
   </si>
   <si>
     <t>["norm:description-list:anchors-in-items:item1", "norm:description-list:anchors-in-items:item3"]</t>
   </si>
   <si>
     <t>desc2</t>
-  </si>
-  <si>
-    <t>rule_with_newlines</t>
-  </si>
-  <si>
-    <t>Here&amp;#8217;s the first line. Here&amp;#8217;s the second line.</t>
-  </si>
-  <si>
-    <t>["norm:tag_with_newlines"]</t>
   </si>
   <si>
     <t>Chapter Name</t>
@@ -592,25 +594,39 @@
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1">
         <f>==
  cell with anchor
 cell without anchor
 ===</f>
         <v>0</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1">
         <f>Header 1|Header 2
 ==
 Cell in column 1, row 1|Cell in column 2, row 1
@@ -618,20 +634,6 @@
 ===</f>
         <v>0</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
@@ -649,24 +651,24 @@
       <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" t="s">
         <v>29</v>
       </c>
     </row>
@@ -678,10 +680,10 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -689,13 +691,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test.adoc to use inline anchors.
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -89,7 +89,7 @@
   </si>
   <si>
     <t>Item 1
- Item 2
+Item 2
 Item 3</t>
   </si>
   <si>
@@ -610,7 +610,7 @@
       </c>
       <c r="C7" s="1">
         <f>==
- cell with anchor
+cell with anchor
 cell without anchor
 ===</f>
         <v>0</v>

</xml_diff>

<commit_message>
Fixes and unit-level tests for issues 106, 107, & 108
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -64,6 +64,15 @@
     <t>["norm:paragraph:inline-anchors:inline-anchor"]</t>
   </si>
   <si>
+    <t>formulae</t>
+  </si>
+  <si>
+    <t>This paragraph looks like a formulae to Excel because it has this &amp;lt; sign in it. Make sure this gets written as a string, not a formulae in the XLSX or else it will create an error in Excel.</t>
+  </si>
+  <si>
+    <t>["norm:formulae"]</t>
+  </si>
+  <si>
     <t>rule_with_newlines</t>
   </si>
   <si>
@@ -76,10 +85,23 @@
     <t>table1</t>
   </si>
   <si>
+    <t>===
+cell with anchor
+cell without anchor
+===</t>
+  </si>
+  <si>
     <t>["norm:table:anchors-in-cells:entire-table"]</t>
   </si>
   <si>
     <t>table2</t>
+  </si>
+  <si>
+    <t>Header 1|Header 2
+===
+Cell in column 1, row 1|Cell in column 2, row 1
+Cell in column 1, row 2|Cell in column 2, row 2
+===</t>
   </si>
   <si>
     <t>["norm:table:no-anchors-in-cells:entire-table"]</t>
@@ -192,8 +214,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0">
+  <autoFilter ref="A1:F12"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -491,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,22 +529,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -608,15 +630,11 @@
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1">
-        <f>==
-cell with anchor
-cell without anchor
-===</f>
-        <v>0</v>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -624,18 +642,13 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1">
-        <f>Header 1|Header 2
-==
-Cell in column 1, row 1|Cell in column 2, row 1
-Cell in column 1, row 2|Cell in column 2, row 2
-===</f>
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -643,13 +656,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -657,18 +670,12 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
         <v>29</v>
       </c>
     </row>
@@ -685,19 +692,39 @@
       <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added adoc output format for norm rules
Signed-off-by: James Ball <quic_jameball@quicinc.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -86,8 +86,8 @@
   </si>
   <si>
     <t>===
-cell with anchor
-cell without anchor
+WITH anchor
+WITHOUT anchor
 ===</t>
   </si>
   <si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>["norm:table:no-anchors-in-cells:entire-table"]</t>
+  </si>
+  <si>
+    <t>anchors-in-cells1</t>
+  </si>
+  <si>
+    <t>WITH anchor</t>
+  </si>
+  <si>
+    <t>["norm:table:anchors-in-cells:entire-table-tagged:cell"]</t>
+  </si>
+  <si>
+    <t>anchors-in-cells2</t>
+  </si>
+  <si>
+    <t>ABC DEF</t>
+  </si>
+  <si>
+    <t>["norm:table:anchors-in-cells:entire-table-not-tagged:cell"]</t>
   </si>
   <si>
     <t>unordered1</t>
@@ -214,8 +232,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0">
-  <autoFilter ref="A1:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0">
+  <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -513,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -529,22 +547,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -692,25 +710,19 @@
       <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -718,13 +730,47 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actually just decided it was easier to output native HTML instead of adoc to HTML.
Signed-off-by: James Ball <quic_jameball@quicinc.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -82,13 +82,19 @@
     <t>["norm:paragraph:tag_with_newlines"]</t>
   </si>
   <si>
+    <t>double_tags</t>
+  </si>
+  <si>
+    <t>This paragraph has two tags but we only ever get a tag for norm:def.</t>
+  </si>
+  <si>
+    <t>["norm:def"]</t>
+  </si>
+  <si>
     <t>table1</t>
   </si>
   <si>
-    <t>===
-WITH anchor
-WITHOUT anchor
-===</t>
+    <t>ENTIRE TABLE</t>
   </si>
   <si>
     <t>["norm:table:anchors-in-cells:entire-table"]</t>
@@ -97,17 +103,10 @@
     <t>table2</t>
   </si>
   <si>
-    <t>Header 1|Header 2
-===
-Cell in column 1, row 1|Cell in column 2, row 1
-Cell in column 1, row 2|Cell in column 2, row 2
-===</t>
-  </si>
-  <si>
     <t>["norm:table:no-anchors-in-cells:entire-table"]</t>
   </si>
   <si>
-    <t>anchors-in-cells1</t>
+    <t>table3</t>
   </si>
   <si>
     <t>WITH anchor</t>
@@ -116,7 +115,7 @@
     <t>["norm:table:anchors-in-cells:entire-table-tagged:cell"]</t>
   </si>
   <si>
-    <t>anchors-in-cells2</t>
+    <t>table4</t>
   </si>
   <si>
     <t>ABC DEF</t>
@@ -126,6 +125,17 @@
   </si>
   <si>
     <t>unordered1</t>
+  </si>
+  <si>
+    <t>Item A
+Item B
+Item C</t>
+  </si>
+  <si>
+    <t>["norm:unordered-list:no-anchors-in-items:entire-list"]</t>
+  </si>
+  <si>
+    <t>unordered2</t>
   </si>
   <si>
     <t>Item 1
@@ -136,7 +146,141 @@
     <t>["norm:unordered-list:anchors-in-items:entire-list"]</t>
   </si>
   <si>
-    <t>note_with_2_tags</t>
+    <t>unordered3</t>
+  </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>["norm:unordered-list:anchors-in-items:item1"]</t>
+  </si>
+  <si>
+    <t>unordered4</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>["norm:unordered-list:anchors-in-items:item2"]</t>
+  </si>
+  <si>
+    <t>unordered5</t>
+  </si>
+  <si>
+    <t>Zca and not F
+Zca, Zcf and F (but not D) is specified (RV32 only)
+Zca, Zcf and Zcd if D is specified (RV32 only)
+this configuration excludes Zcmp, Zcmt
+Zca, Zcd if D is specified (RV64 only)
+this configuration excludes Zcmp, Zcmt</t>
+  </si>
+  <si>
+    <t>["norm:unordered-list:multiple-levels"]</t>
+  </si>
+  <si>
+    <t>ordered1</t>
+  </si>
+  <si>
+    <t>["norm:ordered-list:no-anchors-in-items:entire-list"]</t>
+  </si>
+  <si>
+    <t>ordered2</t>
+  </si>
+  <si>
+    <t>["norm:ordered-list:anchors-in-items:entire-list"]</t>
+  </si>
+  <si>
+    <t>ordered3</t>
+  </si>
+  <si>
+    <t>["norm:ordered-list:anchors-in-items:item1"]</t>
+  </si>
+  <si>
+    <t>ordered4</t>
+  </si>
+  <si>
+    <t>["norm:ordered-list:anchors-in-items:item2"]</t>
+  </si>
+  <si>
+    <t>desc1</t>
+  </si>
+  <si>
+    <t>Description-A
+Item A
+Description-B
+Item B
+Description-C
+Item C</t>
+  </si>
+  <si>
+    <t>["norm:description-list:no-anchors-in-items:entire-list"]</t>
+  </si>
+  <si>
+    <t>desc2</t>
+  </si>
+  <si>
+    <t>Description-1</t>
+  </si>
+  <si>
+    <t>["norm:description-list:anchors-in-items:entire-list"]</t>
+  </si>
+  <si>
+    <t>desc3</t>
+  </si>
+  <si>
+    <t>Item 1
+Item 3</t>
+  </si>
+  <si>
+    <t>["norm:description-list:anchors-in-items:item1", "norm:description-list:anchors-in-items:item3"]</t>
+  </si>
+  <si>
+    <t>desc4</t>
+  </si>
+  <si>
+    <t>admon1</t>
+  </si>
+  <si>
+    <t>Single paragraph note
+that spans lines.</t>
+  </si>
+  <si>
+    <t>["norm:admonition:single-paragraph-note"]</t>
+  </si>
+  <si>
+    <t>admon2</t>
+  </si>
+  <si>
+    <t>Paragraph A
+Paragraph B
+Paragraph C</t>
+  </si>
+  <si>
+    <t>["norm:admonition:no-anchors-in-notes:entire-note"]</t>
+  </si>
+  <si>
+    <t>admon3</t>
+  </si>
+  <si>
+    <t>Paragraph 1
+Paragraph 2
+Paragraph 3</t>
+  </si>
+  <si>
+    <t>["norm:admonition:anchors-in-notes:entire-note"]</t>
+  </si>
+  <si>
+    <t>admon4</t>
+  </si>
+  <si>
+    <t>Paragraph X
+Paragraph Z</t>
+  </si>
+  <si>
+    <t>["norm:admonition:only-anchors-in-notes:note1", "norm:admonition:only-anchors-in-notes:note3"]</t>
+  </si>
+  <si>
+    <t>admon5</t>
   </si>
   <si>
     <t>One line description
@@ -151,19 +295,6 @@
   </si>
   <si>
     <t>MY_PARAMETER</t>
-  </si>
-  <si>
-    <t>desc1</t>
-  </si>
-  <si>
-    <t>Item 1
-Item 3</t>
-  </si>
-  <si>
-    <t>["norm:description-list:anchors-in-items:item1", "norm:description-list:anchors-in-items:item3"]</t>
-  </si>
-  <si>
-    <t>desc2</t>
   </si>
   <si>
     <t>Chapter Name</t>
@@ -232,8 +363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0">
-  <autoFilter ref="A1:F14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0">
+  <autoFilter ref="A1:F29"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -531,7 +662,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -547,22 +678,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -691,10 +822,10 @@
         <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -702,13 +833,13 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -716,13 +847,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -730,19 +861,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -750,13 +875,13 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -764,13 +889,229 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made norm rule HTML sidebar more compact and display truncated tables
Signed-off-by: James Ball <quic_jameball@quicinc.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -94,7 +94,10 @@
     <t>table1</t>
   </si>
   <si>
-    <t>ENTIRE TABLE</t>
+    <t>===
+WITH anchor
+WITHOUT anchor
+===</t>
   </si>
   <si>
     <t>["norm:table:anchors-in-cells:entire-table"]</t>
@@ -103,6 +106,13 @@
     <t>table2</t>
   </si>
   <si>
+    <t>Header 1|Header 2
+===
+Cell in column 1, row 1|Cell in column 2, row 1
+Cell in column 1, row 2|Cell in column 2, row 2
+===</t>
+  </si>
+  <si>
     <t>["norm:table:no-anchors-in-cells:entire-table"]</t>
   </si>
   <si>
@@ -122,6 +132,28 @@
   </si>
   <si>
     <t>["norm:table:anchors-in-cells:entire-table-not-tagged:cell"]</t>
+  </si>
+  <si>
+    <t>table5</t>
+  </si>
+  <si>
+    <t>Name|Color
+===
+Roses|Red
+Violets|Blue
+Name1|Color1
+Name2|Color2
+Name3|Color3
+Name4|Color4
+Name5|Color5
+Name6|Color6
+Name7|Color8
+Name9|Color9
+Name10|Color10
+...</t>
+  </si>
+  <si>
+    <t>["norm:table:many-rows"]</t>
   </si>
   <si>
     <t>unordered1</t>
@@ -363,8 +395,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0">
-  <autoFilter ref="A1:F29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F30" totalsRowShown="0">
+  <autoFilter ref="A1:F30"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -662,7 +694,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -678,22 +710,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -822,10 +854,10 @@
         <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -833,13 +865,13 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -847,13 +879,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -861,13 +893,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -875,13 +907,13 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -889,13 +921,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -903,13 +935,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -917,13 +949,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -931,13 +963,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -945,13 +977,13 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -959,13 +991,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -973,13 +1005,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -987,13 +1019,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1001,13 +1033,13 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1015,13 +1047,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1029,13 +1061,13 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1043,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>69</v>
@@ -1057,13 +1089,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1071,13 +1103,13 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1085,13 +1117,13 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1099,19 +1131,33 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" t="s">
         <v>83</v>
       </c>
-      <c r="F30" t="s">
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>84</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow instance and tag (not always requiring instances and tags). Cleanup JSON schema definition to get better error checking.
Signed-off-by: James Ball <quic_jameball@quicinc.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Zicsr, ABC</t>
+  </si>
+  <si>
+    <t>no_tag</t>
+  </si>
+  <si>
+    <t>Normative rule without tag/tags</t>
+  </si>
+  <si>
+    <t>Summary</t>
   </si>
   <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
@@ -324,9 +333,6 @@
   </si>
   <si>
     <t>parameter</t>
-  </si>
-  <si>
-    <t>MY_PARAMETER</t>
   </si>
   <si>
     <t>Chapter Name</t>
@@ -395,8 +401,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F30" totalsRowShown="0">
-  <autoFilter ref="A1:F30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0">
+  <autoFilter ref="A1:F31"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -694,7 +700,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -705,27 +711,27 @@
     <col min="3" max="3" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -944,7 +950,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -958,7 +964,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -972,7 +978,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -980,69 +986,69 @@
         <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1078,27 +1084,27 @@
         <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1153,11 +1159,22 @@
       <c r="D31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E31" t="s">
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F31" t="s">
+      <c r="C32" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Display kind and instances and rename ADOC/HTML columns to better match variety of content.
Signed-off-by: James Ball <quic_jameball@quicinc.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="98">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>parameter</t>
+  </si>
+  <si>
+    <t>MY_PARAMETER</t>
   </si>
   <si>
     <t>Chapter Name</t>
@@ -711,27 +714,27 @@
     <col min="3" max="3" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -950,7 +953,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -964,7 +967,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -978,7 +981,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -992,7 +995,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1175,6 +1178,9 @@
       </c>
       <c r="E32" t="s">
         <v>90</v>
+      </c>
+      <c r="F32" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename norm rule table columns and documentation on how to tag normative text with a # in it.
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -26,7 +26,7 @@
 inside inline</t>
   </si>
   <si>
-    <t>Summary, ["norm:inline"]</t>
+    <t>Rule Summary, ["norm:inline"]</t>
   </si>
   <si>
     <t>extension</t>
@@ -41,7 +41,16 @@
     <t>Normative rule without tag/tags</t>
   </si>
   <si>
-    <t>Summary</t>
+    <t>Rule Summary</t>
+  </si>
+  <si>
+    <t>inline-with-hash</t>
+  </si>
+  <si>
+    <t>includes a hash # symbol.</t>
+  </si>
+  <si>
+    <t>["norm:inline-with-hash"]</t>
   </si>
   <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
@@ -52,7 +61,7 @@
 Paragraph without inline anchors</t>
   </si>
   <si>
-    <t>Description, ["norm:paragraph:no-inline-anchors"]</t>
+    <t>Rule Description, ["norm:paragraph:no-inline-anchors"]</t>
   </si>
   <si>
     <t>inline-anchors-in-paragraph-entire</t>
@@ -329,7 +338,7 @@
 Paragraph 3</t>
   </si>
   <si>
-    <t>Description, ["norm:admonition:anchors-in-notes:note1", "norm:admonition:anchors-in-notes:note3"]</t>
+    <t>Rule Description, ["norm:admonition:anchors-in-notes:note1", "norm:admonition:anchors-in-notes:note3"]</t>
   </si>
   <si>
     <t>parameter</t>
@@ -344,10 +353,10 @@
     <t>Rule Name</t>
   </si>
   <si>
-    <t>Rule Definition</t>
-  </si>
-  <si>
-    <t>Rule Definition Sources</t>
+    <t>Rule Description</t>
+  </si>
+  <si>
+    <t>Description Location</t>
   </si>
   <si>
     <t>Kind</t>
@@ -404,13 +413,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0">
-  <autoFilter ref="A1:F31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F32" totalsRowShown="0">
+  <autoFilter ref="A1:F32"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
-    <tableColumn id="3" name="Rule Definition"/>
-    <tableColumn id="4" name="Rule Definition Sources"/>
+    <tableColumn id="3" name="Rule Description"/>
+    <tableColumn id="4" name="Description Location"/>
     <tableColumn id="5" name="Kind"/>
     <tableColumn id="6" name="Instances"/>
   </tableColumns>
@@ -703,7 +712,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -719,22 +728,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -953,7 +962,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -967,7 +976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -981,7 +990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -995,7 +1004,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1003,69 +1012,69 @@
         <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1088,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +1102,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1101,27 +1110,27 @@
         <v>74</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1144,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1158,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1172,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1176,11 +1185,25 @@
       <c r="D32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E32" t="s">
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F32" t="s">
+      <c r="C33" s="1" t="s">
         <v>91</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tests for norm rules with Unicode character sequences inside norm rules.
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -23,7 +23,7 @@
   </si>
   <si>
     <t>A few words
-inside inline</t>
+inside &amp;gt; &amp;amp;gt; inline</t>
   </si>
   <si>
     <t>Rule Summary, ["norm:inline"]</t>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Zicsr, ABC</t>
+  </si>
+  <si>
+    <t>infinity</t>
+  </si>
+  <si>
+    <t>abc &amp;amp;#x221e; def</t>
+  </si>
+  <si>
+    <t>["norm:infinity"]</t>
   </si>
   <si>
     <t>no_tag</t>
@@ -413,8 +422,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F32" totalsRowShown="0">
-  <autoFilter ref="A1:F32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F33" totalsRowShown="0">
+  <autoFilter ref="A1:F33"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -712,7 +721,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -728,22 +737,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1026,10 +1035,10 @@
         <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1037,13 +1046,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1051,13 +1060,13 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1065,13 +1074,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1079,10 +1088,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>70</v>
@@ -1124,10 +1133,10 @@
         <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1135,13 +1144,13 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1199,11 +1208,25 @@
       <c r="D33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E33" t="s">
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F33" t="s">
+      <c r="C34" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert adoc in tags to HTML for everything except adoc macro calls (e.g., 100 {le} 200).
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -23,7 +23,7 @@
   </si>
   <si>
     <t>A few words
-inside &amp;gt; &amp;amp;gt; inline</t>
+inside inline</t>
   </si>
   <si>
     <t>Rule Summary, ["norm:inline"]</t>
@@ -33,15 +33,6 @@
   </si>
   <si>
     <t>Zicsr, ABC</t>
-  </si>
-  <si>
-    <t>infinity</t>
-  </si>
-  <si>
-    <t>abc &amp;amp;#x221e; def</t>
-  </si>
-  <si>
-    <t>["norm:infinity"]</t>
   </si>
   <si>
     <t>no_tag</t>
@@ -116,6 +107,87 @@
   </si>
   <si>
     <t>["norm:def"]</t>
+  </si>
+  <si>
+    <t>superscript</t>
+  </si>
+  <si>
+    <t>xyz 2^32^ 123</t>
+  </si>
+  <si>
+    <t>["norm:superscript"]</t>
+  </si>
+  <si>
+    <t>subscript</t>
+  </si>
+  <si>
+    <t>xyz X~i~ 123</t>
+  </si>
+  <si>
+    <t>["norm:subscript"]</t>
+  </si>
+  <si>
+    <t>inline-underline</t>
+  </si>
+  <si>
+    <t>ABC [.underline]#inside tag# GHI</t>
+  </si>
+  <si>
+    <t>["norm:inline-underline"]</t>
+  </si>
+  <si>
+    <t>paragraph-underline</t>
+  </si>
+  <si>
+    <t>Paragraph underlined outside.</t>
+  </si>
+  <si>
+    <t>["norm:paragraph-underline"]</t>
+  </si>
+  <si>
+    <t>unicode_name</t>
+  </si>
+  <si>
+    <t>ABC &amp;amp;ge; DEF</t>
+  </si>
+  <si>
+    <t>["norm:unicode_name"]</t>
+  </si>
+  <si>
+    <t>unicode_decimal_value</t>
+  </si>
+  <si>
+    <t>ABC &amp;amp;#8805; DEF</t>
+  </si>
+  <si>
+    <t>["norm:unicode_decimal_value"]</t>
+  </si>
+  <si>
+    <t>unicode_hexadecimal_value</t>
+  </si>
+  <si>
+    <t>ABC &amp;amp;#x2265; DEF</t>
+  </si>
+  <si>
+    <t>["norm:unicode_hexadecimal_value"]</t>
+  </si>
+  <si>
+    <t>unicode_char</t>
+  </si>
+  <si>
+    <t>ABC ≥ DEF</t>
+  </si>
+  <si>
+    <t>["norm:unicode_char"]</t>
+  </si>
+  <si>
+    <t>macro_call</t>
+  </si>
+  <si>
+    <t>200 {ge} 100</t>
+  </si>
+  <si>
+    <t>["norm:macro_call"]</t>
   </si>
   <si>
     <t>table1</t>
@@ -365,7 +437,7 @@
     <t>Rule Description</t>
   </si>
   <si>
-    <t>Description Location</t>
+    <t>Origin of Description</t>
   </si>
   <si>
     <t>Kind</t>
@@ -422,13 +494,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F33" totalsRowShown="0">
-  <autoFilter ref="A1:F33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
+  <autoFilter ref="A1:F41"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
     <tableColumn id="3" name="Rule Description"/>
-    <tableColumn id="4" name="Description Location"/>
+    <tableColumn id="4" name="Origin of Description"/>
     <tableColumn id="5" name="Kind"/>
     <tableColumn id="6" name="Instances"/>
   </tableColumns>
@@ -721,7 +793,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -737,22 +809,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1049,10 +1121,10 @@
         <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1060,13 +1132,13 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1074,13 +1146,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1088,13 +1160,13 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1102,13 +1174,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1116,13 +1188,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1130,13 +1202,13 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1144,13 +1216,13 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1158,13 +1230,13 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1172,13 +1244,13 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1186,13 +1258,13 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1200,13 +1272,13 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1214,19 +1286,131 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E42" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for normative tag hyperlinks in normatively tagged text.
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -145,10 +145,19 @@
     <t>["norm:paragraph-underline"]</t>
   </si>
   <si>
+    <t>standalone_ampersand</t>
+  </si>
+  <si>
+    <t>ABC &amp;amp; DEF</t>
+  </si>
+  <si>
+    <t>["norm:standalone_ampersand"]</t>
+  </si>
+  <si>
     <t>unicode_name</t>
   </si>
   <si>
-    <t>ABC &amp;amp;ge; DEF</t>
+    <t>DEF &amp;amp;ge; GHI</t>
   </si>
   <si>
     <t>["norm:unicode_name"]</t>
@@ -157,7 +166,7 @@
     <t>unicode_decimal_value</t>
   </si>
   <si>
-    <t>ABC &amp;amp;#8805; DEF</t>
+    <t>GHI &amp;amp;#8805; JKL</t>
   </si>
   <si>
     <t>["norm:unicode_decimal_value"]</t>
@@ -166,7 +175,7 @@
     <t>unicode_hexadecimal_value</t>
   </si>
   <si>
-    <t>ABC &amp;amp;#x2265; DEF</t>
+    <t>JKL &amp;amp;#x2265; MNO</t>
   </si>
   <si>
     <t>["norm:unicode_hexadecimal_value"]</t>
@@ -175,7 +184,7 @@
     <t>unicode_char</t>
   </si>
   <si>
-    <t>ABC ≥ DEF</t>
+    <t>MNO ≥ PQR</t>
   </si>
   <si>
     <t>["norm:unicode_char"]</t>
@@ -188,6 +197,24 @@
   </si>
   <si>
     <t>["norm:macro_call"]</t>
+  </si>
+  <si>
+    <t>hyperlink1</t>
+  </si>
+  <si>
+    <t>ABC &amp;lt;&amp;lt;norm:superscript&amp;gt;&amp;gt; DEF</t>
+  </si>
+  <si>
+    <t>["norm:hyperlink1"]</t>
+  </si>
+  <si>
+    <t>hyperlink2</t>
+  </si>
+  <si>
+    <t>DEF &amp;lt;&amp;lt;norm:superscript,custom text&amp;gt;&amp;gt; GHI</t>
+  </si>
+  <si>
+    <t>["norm:hyperlink2"]</t>
   </si>
   <si>
     <t>table1</t>
@@ -425,7 +452,7 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>MY_PARAMETER</t>
+    <t>my_parameter</t>
   </si>
   <si>
     <t>Chapter Name</t>
@@ -494,8 +521,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
-  <autoFilter ref="A1:F41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F44" totalsRowShown="0">
+  <autoFilter ref="A1:F44"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -793,7 +820,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -804,27 +831,27 @@
     <col min="3" max="3" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1233,10 +1260,10 @@
         <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1244,13 +1271,13 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1258,13 +1285,13 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1272,13 +1299,13 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1286,13 +1313,13 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1300,13 +1327,13 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1314,10 +1341,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>103</v>
@@ -1331,10 +1358,10 @@
         <v>104</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1342,13 +1369,13 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1356,13 +1383,13 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1370,13 +1397,13 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1406,11 +1433,53 @@
       <c r="D42" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E42" t="s">
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F42" t="s">
+      <c r="C43" s="1" t="s">
         <v>121</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now handle any <<foo>> or <<foo,link text> anchor in norm rules
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="143">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -215,6 +215,24 @@
   </si>
   <si>
     <t>["norm:hyperlink2"]</t>
+  </si>
+  <si>
+    <t>hyperlink3</t>
+  </si>
+  <si>
+    <t>ABC &amp;lt;&amp;lt;non-norm-anchor&amp;gt;&amp;gt; DEF</t>
+  </si>
+  <si>
+    <t>["norm:hyperlink3"]</t>
+  </si>
+  <si>
+    <t>hyperlink4</t>
+  </si>
+  <si>
+    <t>DEF &amp;lt;&amp;lt;non-norm-anchor,custom text&amp;gt;&amp;gt; GHI</t>
+  </si>
+  <si>
+    <t>["norm:hyperlink4"]</t>
   </si>
   <si>
     <t>table1</t>
@@ -521,8 +539,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F44" totalsRowShown="0">
-  <autoFilter ref="A1:F44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0">
+  <autoFilter ref="A1:F46"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -820,7 +838,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -836,22 +854,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1302,10 +1320,10 @@
         <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1313,13 +1331,13 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1327,13 +1345,13 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1341,13 +1359,13 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>91</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1355,13 +1373,13 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1369,10 +1387,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>109</v>
@@ -1400,10 +1418,10 @@
         <v>113</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1411,13 +1429,13 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1425,13 +1443,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1475,11 +1493,39 @@
       <c r="D45" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E45" t="s">
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F45" t="s">
+      <c r="C46" s="1" t="s">
         <v>130</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for having two or more links in normative text
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="149">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -233,6 +233,24 @@
   </si>
   <si>
     <t>["norm:hyperlink4"]</t>
+  </si>
+  <si>
+    <t>hyperlink5</t>
+  </si>
+  <si>
+    <t>GHI &amp;lt;&amp;lt;norm:superscript&amp;gt;&amp;gt; and &amp;lt;&amp;lt;norm:subscript&amp;gt;&amp;gt; JKL</t>
+  </si>
+  <si>
+    <t>["norm:hyperlink5"]</t>
+  </si>
+  <si>
+    <t>hyperlink6</t>
+  </si>
+  <si>
+    <t>JKL &amp;lt;&amp;lt;norm:superscript,hello&amp;gt;&amp;gt; and &amp;lt;&amp;lt;norm:subscript,goodbye&amp;gt;&amp;gt; MNO</t>
+  </si>
+  <si>
+    <t>["norm:hyperlink6"]</t>
   </si>
   <si>
     <t>table1</t>
@@ -539,8 +557,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0">
-  <autoFilter ref="A1:F46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F48" totalsRowShown="0">
+  <autoFilter ref="A1:F48"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -838,7 +856,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -854,22 +872,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1312,7 +1330,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1344,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1358,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1348,83 +1366,83 @@
         <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>97</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +1456,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1446,41 +1464,41 @@
         <v>119</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1494,7 +1512,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1508,7 +1526,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -1521,11 +1539,39 @@
       <c r="D47" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E47" t="s">
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F47" t="s">
+      <c r="C48" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert adoc tables to html tables
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -257,8 +257,8 @@
   </si>
   <si>
     <t>===
-WITH anchor
-WITHOUT anchor
+|WITH anchor
+|WITHOUT anchor
 ===</t>
   </si>
   <si>
@@ -268,10 +268,10 @@
     <t>table2</t>
   </si>
   <si>
-    <t>Header 1|Header 2
+    <t>|Header 1|Header 2
 ===
-Cell in column 1, row 1|Cell in column 2, row 1
-Cell in column 1, row 2|Cell in column 2, row 2
+|Cell in column 1, row 1|Cell in column 2, row 1
+|Cell in column 1, row 2|Cell in column 2, row 2
 ===</t>
   </si>
   <si>
@@ -299,19 +299,19 @@
     <t>table5</t>
   </si>
   <si>
-    <t>Name|Color
+    <t>|Name|Color
 ===
-Roses|Red
-Violets|Blue
-Name1|Color1
-Name2|Color2
-Name3|Color3
-Name4|Color4
-Name5|Color5
-Name6|Color6
-Name7|Color8
-Name9|Color9
-Name10|Color10
+|Roses|Red
+|Violets|Blue
+|Name1|Color1
+|Name2|Color2
+|Name3|Color3
+|Name4|Color4
+|Name5|Color5
+|Name6|Color6
+|Name7|Color7
+|Name8|Color8
+|Name9|Color9
 ...</t>
   </si>
   <si>

</xml_diff>

<commit_message>
Reverted tags backend to just joining table cells with "|" (was for a while prefixing each cell with "|"), changed norm rules Ruby to use split() function instead of complicated regular expression that wasn't robust. Added test case for single char table cells (would have failed before).
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="152">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -257,8 +257,8 @@
   </si>
   <si>
     <t>===
-|WITH anchor
-|WITHOUT anchor
+WITH anchor
+WITHOUT anchor
 ===</t>
   </si>
   <si>
@@ -268,10 +268,10 @@
     <t>table2</t>
   </si>
   <si>
-    <t>|Header 1|Header 2
+    <t>Header 1|Header 2
 ===
-|Cell in column 1, row 1|Cell in column 2, row 1
-|Cell in column 1, row 2|Cell in column 2, row 2
+Cell in column 1, row 1|Cell in column 2, row 1
+Cell in column 1, row 2|Cell in column 2, row 2
 ===</t>
   </si>
   <si>
@@ -299,23 +299,36 @@
     <t>table5</t>
   </si>
   <si>
-    <t>|Name|Color
+    <t>Name|Color
 ===
-|Roses|Red
-|Violets|Blue
-|Name1|Color1
-|Name2|Color2
-|Name3|Color3
-|Name4|Color4
-|Name5|Color5
-|Name6|Color6
-|Name7|Color7
-|Name8|Color8
-|Name9|Color9
+Roses|Red
+Violets|Blue
+Name1|Color1
+Name2|Color2
+Name3|Color3
+Name4|Color4
+Name5|Color5
+Name6|Color6
+Name7|Color7
+Name8|Color8
+Name9|Color9
 ...</t>
   </si>
   <si>
     <t>["norm:table:many-rows"]</t>
+  </si>
+  <si>
+    <t>table6</t>
+  </si>
+  <si>
+    <t>X1|X2
+===
+A|B
+C|D
+===</t>
+  </si>
+  <si>
+    <t>["norm:table:single-char-cells"]</t>
   </si>
   <si>
     <t>unordered1</t>
@@ -557,8 +570,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F48" totalsRowShown="0">
-  <autoFilter ref="A1:F48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F49" totalsRowShown="0">
+  <autoFilter ref="A1:F49"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -856,7 +869,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -872,22 +885,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1394,10 +1407,10 @@
         <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1405,13 +1418,13 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>97</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1419,13 +1432,13 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1433,13 +1446,13 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1447,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>118</v>
@@ -1492,10 +1505,10 @@
         <v>125</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1503,13 +1516,13 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1567,11 +1580,25 @@
       <c r="D49" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E49" t="s">
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F49" t="s">
+      <c r="C50" s="1" t="s">
         <v>142</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" t="s">
+        <v>144</v>
+      </c>
+      <c r="F50" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added note keyword and added to unit test
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -38,10 +38,11 @@
     <t>no_tag</t>
   </si>
   <si>
-    <t>Normative rule without tag/tags</t>
-  </si>
-  <si>
-    <t>Rule Summary</t>
+    <t>Normative rule without tag/tags
+This normative rule has no references to the standard. This should only be used in extraordinary circumstances.</t>
+  </si>
+  <si>
+    <t>Rule Summary, Rule Note</t>
   </si>
   <si>
     <t>inline-with-hash</t>
@@ -247,7 +248,7 @@
     <t>hyperlink6</t>
   </si>
   <si>
-    <t>JKL &amp;lt;&amp;lt;norm:superscript,hello&amp;gt;&amp;gt; and &amp;lt;&amp;lt;norm:subscript,goodbye&amp;gt;&amp;gt; MNO</t>
+    <t>JKL &amp;lt;&amp;lt;norm:superscript ,hello&amp;gt;&amp;gt; and &amp;lt;&amp;lt;norm:subscript, goodbye&amp;gt;&amp;gt; MNO</t>
   </si>
   <si>
     <t>["norm:hyperlink6"]</t>

</xml_diff>

<commit_message>
Added ability for note/description/summary to link to other normative rules. Also added adoc to HTML improvements based on better knowledge of adoc.
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="158">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -38,8 +38,11 @@
     <t>no_tag</t>
   </si>
   <si>
-    <t>Normative rule without tag/tags
-This normative rule has no references to the standard. This should only be used in extraordinary circumstances.</t>
+    <t>Normative rule *without* tag/tags
+This normative rule has no references to the standard. This should only be used in extraordinary circumstances.
+It does include a link to &lt;&lt;table1&gt;&gt; (another normative rule).
+Has basic adoc formatting such as *bold*, ita__lics__, `monospace`, 2^superscript^, ~subscript~, [.underline]#underline#,
+and &amp;le; (Unicode text for less-than-equals-to) and &amp;#8800; (Unicode decimal value for not-equal-to).</t>
   </si>
   <si>
     <t>Rule Summary, Rule Note</t>
@@ -57,7 +60,7 @@
     <t>paragraph-with-a-really-wide-rule-name</t>
   </si>
   <si>
-    <t>Here's a description.
+    <t>Here's a [.underline]#description#.
 It's got 2 lines.
 Paragraph without inline anchors</t>
   </si>
@@ -110,10 +113,28 @@
     <t>["norm:def"]</t>
   </si>
   <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>ABC is a network - Bold is removed by tags backend so I don't see it</t>
+  </si>
+  <si>
+    <t>["norm:bold"]</t>
+  </si>
+  <si>
+    <t>italics</t>
+  </si>
+  <si>
+    <t>Let's have fun today - Italics is removed by tags backend so I don't see it</t>
+  </si>
+  <si>
+    <t>["norm:italics"]</t>
+  </si>
+  <si>
     <t>superscript</t>
   </si>
   <si>
-    <t>xyz 2^32^ 123</t>
+    <t>both 2^32^ and ^32^ work</t>
   </si>
   <si>
     <t>["norm:superscript"]</t>
@@ -122,7 +143,7 @@
     <t>subscript</t>
   </si>
   <si>
-    <t>xyz X~i~ 123</t>
+    <t>both ~log~ and log~2~ work</t>
   </si>
   <si>
     <t>["norm:subscript"]</t>
@@ -571,8 +592,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F49" totalsRowShown="0">
-  <autoFilter ref="A1:F49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F51" totalsRowShown="0">
+  <autoFilter ref="A1:F51"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -870,7 +891,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -886,22 +907,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1422,10 +1443,10 @@
         <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1433,13 +1454,13 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1447,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1461,13 +1482,13 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1475,13 +1496,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1489,10 +1510,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>124</v>
@@ -1520,10 +1541,10 @@
         <v>128</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1531,13 +1552,13 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1545,13 +1566,13 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1595,11 +1616,39 @@
       <c r="D50" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E50" t="s">
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F50" t="s">
+      <c r="C51" s="1" t="s">
         <v>145</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" t="s">
+        <v>150</v>
+      </c>
+      <c r="F52" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issues in adoc to HTML formatting found by Copilot review
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -38,14 +38,15 @@
     <t>no_tag</t>
   </si>
   <si>
-    <t>Normative rule *without* tag/tags
+    <t>Normative rule *without* tag/tags and *nested **bold** cases*.
 This normative rule has no references to the standard. This should only be used in extraordinary circumstances.
 It does include a link to &lt;&lt;table1&gt;&gt; (another normative rule).
 Has basic adoc formatting such as *bold*, ita__lics__, `monospace`, 2^superscript^, ~subscript~, [.underline]#underline#,
-and &amp;le; (Unicode text for less-than-equals-to) and &amp;#8800; (Unicode decimal value for not-equal-to).</t>
-  </si>
-  <si>
-    <t>Rule Summary, Rule Note</t>
+and &amp;le; (Unicode text for less-than-equals-to) and &amp;#8800; (Unicode decimal value for not-equal-to).
+Let's try a nested *_bold italics_* case or all 3 *_`bold italic monospace`_* too.</t>
+  </si>
+  <si>
+    <t>Rule Summary, Rule Note, Rule Description</t>
   </si>
   <si>
     <t>inline-with-hash</t>

</xml_diff>

<commit_message>
Use paragraph symbol to separate adoc table rows
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="161">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -280,8 +280,7 @@
   </si>
   <si>
     <t>===
-WITH anchor
-WITHOUT anchor
+WITH anchor¶WITHOUT anchor
 ===</t>
   </si>
   <si>
@@ -293,8 +292,7 @@
   <si>
     <t>Header 1|Header 2
 ===
-Cell in column 1, row 1|Cell in column 2, row 1
-Cell in column 1, row 2|Cell in column 2, row 2
+Cell in column 1, row 1|Cell in column 2, row 1¶Cell in column 1, row 2|Cell in column 2, row 2
 ===</t>
   </si>
   <si>
@@ -324,18 +322,8 @@
   <si>
     <t>Name|Color
 ===
-Roses|Red
-Violets|Blue
-Name1|Color1
-Name2|Color2
-Name3|Color3
-Name4|Color4
-Name5|Color5
-Name6|Color6
-Name7|Color7
-Name8|Color8
-Name9|Color9
-...</t>
+Roses|Red¶Violets|Blue¶Name1|Color1¶Name2|Color2¶Name3|Color3¶Name4|Color4¶Name5|Color5¶Name6|Color6¶Name7|Color7¶Name8|Color8¶Name9|Color9¶Name10|Color10¶Name11|Color11¶Name12|Color12¶Name13|Color13¶Name14|Color14
+===</t>
   </si>
   <si>
     <t>["norm:table:many-rows"]</t>
@@ -346,12 +334,25 @@
   <si>
     <t>X1|X2
 ===
-A|B
-C|D
+A|B¶C|D
 ===</t>
   </si>
   <si>
     <t>["norm:table:single-char-cells"]</t>
+  </si>
+  <si>
+    <t>table7</t>
+  </si>
+  <si>
+    <t>ColA|ColB
+===
+0
+1|Off
+On
+===</t>
+  </si>
+  <si>
+    <t>["norm:table:column-first-order"]</t>
   </si>
   <si>
     <t>unordered1</t>
@@ -593,8 +594,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F51" totalsRowShown="0">
-  <autoFilter ref="A1:F51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F52" totalsRowShown="0">
+  <autoFilter ref="A1:F52"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -892,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -908,22 +909,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1472,10 +1473,10 @@
         <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1483,13 +1484,13 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1497,13 +1498,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1511,13 +1512,13 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1525,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>127</v>
@@ -1570,10 +1571,10 @@
         <v>134</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1581,13 +1582,13 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1645,11 +1646,25 @@
       <c r="D52" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E52" t="s">
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F52" t="s">
+      <c r="C53" s="1" t="s">
         <v>151</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E53" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added clarification-text and clarification-link to norm rule defs.
Signed-off-by: James Ball <quic_jameball@quicinc.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="167">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>["norm:inline-with-hash"]</t>
+  </si>
+  <si>
+    <t>clarification-without-text</t>
+  </si>
+  <si>
+    <t>https://www.github.com/riscv/jfkd/issues/67
+isn't clear enough.</t>
+  </si>
+  <si>
+    <t>Rule Clarification Link, ["norm:clarification-without-text"]</t>
+  </si>
+  <si>
+    <t>clarification-with-text</t>
+  </si>
+  <si>
+    <t>https://github.com/riscv/jfkd/issues/67
+This is the optional clarifying text.
+also isn't clear enough.</t>
+  </si>
+  <si>
+    <t>Rule Clarification Link, Rule Clarification Text, ["norm:clarification-with-text"]</t>
   </si>
   <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
@@ -594,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F52" totalsRowShown="0">
-  <autoFilter ref="A1:F52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0">
+  <autoFilter ref="A1:F54"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -893,7 +914,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -909,22 +930,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1487,10 +1508,10 @@
         <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1498,13 +1519,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1512,13 +1533,13 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1526,13 +1547,13 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1540,13 +1561,13 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1554,10 +1575,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>133</v>
@@ -1585,10 +1606,10 @@
         <v>137</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1596,13 +1617,13 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1610,13 +1631,13 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1660,11 +1681,39 @@
       <c r="D53" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E53" t="s">
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F53" t="s">
+      <c r="C54" s="1" t="s">
         <v>154</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E55" t="s">
+        <v>159</v>
+      </c>
+      <c r="F55" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"tags" table format now supported
Signed-off-by: James Ball <quic_jameball@quicinc.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="169">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>Rule Clarification Link, Rule Clarification Text, ["norm:clarification-with-text"]</t>
+  </si>
+  <si>
+    <t>clarification-with-table</t>
+  </si>
+  <si>
+    <t>https://github.com/riscv/something/issues/67
+Header1 | Header2
+===
+R1C1   | R1C2¶
+R2C1   | R2C2
+===
+also isn't clear enough.</t>
   </si>
   <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
@@ -615,8 +627,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0">
-  <autoFilter ref="A1:F54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F55" totalsRowShown="0">
+  <autoFilter ref="A1:F55"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -914,7 +926,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -930,22 +942,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1035,7 +1047,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1043,13 +1055,13 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1057,13 +1069,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1071,13 +1083,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1085,13 +1097,13 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1099,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1113,13 +1125,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1127,13 +1139,13 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1141,13 +1153,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1155,13 +1167,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1169,13 +1181,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1183,13 +1195,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1197,13 +1209,13 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1211,13 +1223,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1225,13 +1237,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1239,13 +1251,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1253,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1267,13 +1279,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1281,13 +1293,13 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1295,13 +1307,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1309,13 +1321,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1323,13 +1335,13 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1337,13 +1349,13 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1351,13 +1363,13 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1365,13 +1377,13 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1379,13 +1391,13 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1393,13 +1405,13 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1407,13 +1419,13 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1421,13 +1433,13 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1435,13 +1447,13 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1449,13 +1461,13 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1463,13 +1475,13 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1477,13 +1489,13 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1491,13 +1503,13 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1505,13 +1517,13 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1519,13 +1531,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1533,10 +1545,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>127</v>
@@ -1550,7 +1562,7 @@
         <v>128</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>129</v>
@@ -1564,7 +1576,7 @@
         <v>130</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>131</v>
@@ -1578,7 +1590,7 @@
         <v>132</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>133</v>
@@ -1592,10 +1604,10 @@
         <v>134</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1603,13 +1615,13 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1617,13 +1629,13 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1631,13 +1643,13 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="D50" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1645,13 +1657,13 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1659,13 +1671,13 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1673,13 +1685,13 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1687,13 +1699,13 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1701,19 +1713,33 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E55" t="s">
+      <c r="C56" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F55" t="s">
+      <c r="D56" s="1" t="s">
         <v>160</v>
+      </c>
+      <c r="E56" t="s">
+        <v>161</v>
+      </c>
+      <c r="F56" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Display [CONTEXT] for tag refs marked as context.
Signed-off-by: James Ball <jameball@qti.qualcomm.com>
</commit_message>
<xml_diff>
--- a/tests/norm-rule/expected/test-norm-rules.xlsx
+++ b/tests/norm-rule/expected/test-norm-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="181">
   <si>
     <t>my-chapter_name</t>
   </si>
@@ -89,6 +89,44 @@
 R2C1   | R2C2
 ===
 also isn't clear enough.</t>
+  </si>
+  <si>
+    <t>cat-colors</t>
+  </si>
+  <si>
+    <t>Cats come in many colors.</t>
+  </si>
+  <si>
+    <t>["norm:cat-colors"]</t>
+  </si>
+  <si>
+    <t>cat-claws-one-line-1</t>
+  </si>
+  <si>
+    <t>This kind of animal has claws.
+Cats come in many colors.</t>
+  </si>
+  <si>
+    <t>["norm:cat-claws", "norm:cat-colors"]</t>
+  </si>
+  <si>
+    <t>cat-claws-one-line-2</t>
+  </si>
+  <si>
+    <t>cat-claws-multi-lines-1</t>
+  </si>
+  <si>
+    <t>Cats come in many colors.
+This kind of animal has claws.</t>
+  </si>
+  <si>
+    <t>["norm:cat-colors", "norm:cat-claws"]</t>
+  </si>
+  <si>
+    <t>cat-claws-multi-lines-2</t>
+  </si>
+  <si>
+    <t>cat-claws-multi-lines-3</t>
   </si>
   <si>
     <t>paragraph-with-a-really-wide-rule-name</t>
@@ -627,8 +665,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F55" totalsRowShown="0">
-  <autoFilter ref="A1:F55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F61" totalsRowShown="0">
+  <autoFilter ref="A1:F61"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Chapter Name"/>
     <tableColumn id="2" name="Rule Name"/>
@@ -926,7 +964,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -942,22 +980,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1086,10 +1124,10 @@
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1097,13 +1135,13 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1111,13 +1149,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1125,13 +1163,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1139,13 +1177,13 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1153,13 +1191,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1167,13 +1205,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1181,13 +1219,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1195,13 +1233,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1209,13 +1247,13 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1223,13 +1261,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1237,13 +1275,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1251,13 +1289,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1265,13 +1303,13 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1279,13 +1317,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1293,13 +1331,13 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1307,13 +1345,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1321,13 +1359,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1335,13 +1373,13 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1349,13 +1387,13 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1363,13 +1401,13 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1377,13 +1415,13 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1391,13 +1429,13 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1405,13 +1443,13 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1419,13 +1457,13 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1433,13 +1471,13 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1447,13 +1485,13 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1461,13 +1499,13 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1475,13 +1513,13 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1489,13 +1527,13 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1503,13 +1541,13 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1517,13 +1555,13 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1531,13 +1569,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1545,13 +1583,13 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1559,13 +1597,13 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1573,13 +1611,13 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1587,13 +1625,13 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1601,13 +1639,13 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1615,13 +1653,13 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1629,13 +1667,13 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1643,13 +1681,13 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1657,13 +1695,13 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1671,13 +1709,13 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1685,13 +1723,13 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1699,13 +1737,13 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1713,13 +1751,13 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1727,19 +1765,103 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E56" t="s">
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F56" t="s">
+      <c r="C59" s="1" t="s">
         <v>162</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E62" t="s">
+        <v>173</v>
+      </c>
+      <c r="F62" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>